<commit_message>
Update new function (custom)
</commit_message>
<xml_diff>
--- a/API 정의서.xlsx
+++ b/API 정의서.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yonsei-my.sharepoint.com/personal/jjw0127_o365_yonsei_ac_kr/Documents/I-suscom/0. 연구실일/12. 저탄소/5차년도/4. 유지보수비용, 재료비율 근거자료/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yonsei-my.sharepoint.com/personal/jjw0127_o365_yonsei_ac_kr/Documents/I-suscom/0. 연구실일/12. 저탄소/5차년도/5.  Remodeling_LCC_project (230522)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{C3B04865-27E2-48BA-B211-F10A316B43F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84717D31-223A-4C34-B7F0-E699ADB74C53}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{C3B04865-27E2-48BA-B211-F10A316B43F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B27B526B-CA96-4A62-836F-AE9E1E0C23F7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="인풋" sheetId="1" r:id="rId1"/>
-    <sheet name="아웃풋" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="아웃풋" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="255">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1204,12 +1205,32 @@
     <t>초기투자비용 (Initial Investment Cost, ICC): 리모델링 총 공사비용입니다. (단위: 원)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>실질금리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>명목금리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인플레이션율</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소비자물가 등락률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>예금은행 대출금리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1250,8 +1271,14 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Roboto-Regular"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1270,8 +1297,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1308,11 +1341,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFF0F0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1359,6 +1401,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1380,17 +1434,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1674,11 +1719,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J255"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="4.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="1" customWidth="1"/>
@@ -1693,24 +1738,24 @@
     <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:10" ht="16.5" customHeight="1">
+      <c r="A1" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-    </row>
-    <row r="3" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+    </row>
+    <row r="3" spans="1:10" ht="31.5" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="26"/>
+      <c r="D3" s="18"/>
       <c r="E3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1730,17 +1775,17 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="24">
-        <v>1</v>
-      </c>
-      <c r="B4" s="24" t="s">
+    <row r="4" spans="1:10" ht="32.25" customHeight="1">
+      <c r="A4" s="19">
+        <v>1</v>
+      </c>
+      <c r="B4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="24"/>
+      <c r="D4" s="19"/>
       <c r="E4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1753,17 +1798,17 @@
       <c r="H4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="20" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="144" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24" t="s">
+    <row r="5" spans="1:10" ht="144" customHeight="1">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="24"/>
+      <c r="D5" s="19"/>
       <c r="E5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1776,15 +1821,15 @@
       <c r="H5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="17"/>
-    </row>
-    <row r="6" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24" t="s">
+      <c r="I5" s="21"/>
+    </row>
+    <row r="6" spans="1:10" ht="32.25" customHeight="1">
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="24"/>
+      <c r="D6" s="19"/>
       <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
@@ -1797,15 +1842,15 @@
       <c r="H6" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="I6" s="17"/>
-    </row>
-    <row r="7" spans="1:10" ht="184.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23" t="s">
+      <c r="I6" s="21"/>
+    </row>
+    <row r="7" spans="1:10" ht="184.5" customHeight="1">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="23"/>
+      <c r="D7" s="17"/>
       <c r="E7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1818,20 +1863,20 @@
       <c r="H7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="18"/>
+      <c r="I7" s="22"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="25">
+    <row r="8" spans="1:10" ht="84" customHeight="1">
+      <c r="A8" s="16">
         <v>2</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="25"/>
+      <c r="D8" s="16"/>
       <c r="E8" s="4" t="s">
         <v>1</v>
       </c>
@@ -1844,17 +1889,17 @@
       <c r="H8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="I8" s="23" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="204" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24" t="s">
+    <row r="9" spans="1:10" ht="204" customHeight="1">
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="24"/>
+      <c r="D9" s="19"/>
       <c r="E9" s="1" t="s">
         <v>1</v>
       </c>
@@ -1867,15 +1912,15 @@
       <c r="H9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="20"/>
-    </row>
-    <row r="10" spans="1:10" ht="222" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23" t="s">
+      <c r="I9" s="24"/>
+    </row>
+    <row r="10" spans="1:10" ht="222" customHeight="1">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="23"/>
+      <c r="D10" s="17"/>
       <c r="E10" s="3" t="s">
         <v>1</v>
       </c>
@@ -1888,20 +1933,20 @@
       <c r="H10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I10" s="21"/>
+      <c r="I10" s="25"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="25">
+    <row r="11" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A11" s="16">
         <v>3</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="25"/>
+      <c r="D11" s="16"/>
       <c r="E11" s="1" t="s">
         <v>1</v>
       </c>
@@ -1914,17 +1959,17 @@
       <c r="H11" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="I11" s="19" t="s">
+      <c r="I11" s="23" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="23"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23" t="s">
+    <row r="12" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="23"/>
+      <c r="D12" s="17"/>
       <c r="E12" s="3" t="s">
         <v>1</v>
       </c>
@@ -1937,20 +1982,20 @@
       <c r="H12" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="I12" s="21"/>
+      <c r="I12" s="25"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="25">
+    <row r="13" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A13" s="16">
         <v>4</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="25"/>
+      <c r="D13" s="16"/>
       <c r="E13" s="1" t="s">
         <v>1</v>
       </c>
@@ -1963,17 +2008,17 @@
       <c r="H13" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="I13" s="19" t="s">
+      <c r="I13" s="23" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23" t="s">
+    <row r="14" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="23"/>
+      <c r="D14" s="17"/>
       <c r="E14" s="1" t="s">
         <v>1</v>
       </c>
@@ -1986,20 +2031,20 @@
       <c r="H14" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="I14" s="21"/>
+      <c r="I14" s="25"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="25">
+    <row r="15" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A15" s="16">
         <v>5</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="25"/>
+      <c r="D15" s="16"/>
       <c r="E15" s="4" t="s">
         <v>36</v>
       </c>
@@ -2012,17 +2057,17 @@
       <c r="H15" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="I15" s="19" t="s">
+      <c r="I15" s="23" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23" t="s">
+    <row r="16" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="23"/>
+      <c r="D16" s="17"/>
       <c r="E16" s="3" t="s">
         <v>36</v>
       </c>
@@ -2035,17 +2080,17 @@
       <c r="H16" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="I16" s="21"/>
+      <c r="I16" s="25"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="1:10" ht="84.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="25">
+    <row r="17" spans="1:10" ht="84.75" customHeight="1">
+      <c r="A17" s="16">
         <v>6</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="16" t="s">
         <v>39</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -2063,17 +2108,17 @@
       <c r="H17" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="I17" s="16" t="s">
+      <c r="I17" s="20" t="s">
         <v>210</v>
       </c>
       <c r="J17" s="13" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="24"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
+    <row r="18" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
       <c r="D18" s="1" t="s">
         <v>42</v>
       </c>
@@ -2089,15 +2134,15 @@
       <c r="H18" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="I18" s="17"/>
+      <c r="I18" s="21"/>
       <c r="J18" s="8" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="24"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
+    <row r="19" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
       <c r="D19" s="1" t="s">
         <v>43</v>
       </c>
@@ -2113,15 +2158,15 @@
       <c r="H19" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="I19" s="17"/>
+      <c r="I19" s="21"/>
       <c r="J19" s="8" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="24"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24" t="s">
+    <row r="20" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19" t="s">
         <v>40</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -2139,15 +2184,15 @@
       <c r="H20" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="I20" s="17"/>
+      <c r="I20" s="21"/>
       <c r="J20" s="8" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="24"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
+    <row r="21" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
       <c r="D21" s="1" t="s">
         <v>42</v>
       </c>
@@ -2163,15 +2208,15 @@
       <c r="H21" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="I21" s="17"/>
+      <c r="I21" s="21"/>
       <c r="J21" s="8" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="24"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
+    <row r="22" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
       <c r="D22" s="1" t="s">
         <v>43</v>
       </c>
@@ -2187,15 +2232,15 @@
       <c r="H22" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="I22" s="17"/>
+      <c r="I22" s="21"/>
       <c r="J22" s="8" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="24"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24" t="s">
+    <row r="23" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19" t="s">
         <v>44</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -2213,15 +2258,15 @@
       <c r="H23" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="I23" s="17"/>
+      <c r="I23" s="21"/>
       <c r="J23" s="8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="24"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
+    <row r="24" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
       <c r="D24" s="1" t="s">
         <v>42</v>
       </c>
@@ -2237,15 +2282,15 @@
       <c r="H24" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="I24" s="17"/>
+      <c r="I24" s="21"/>
       <c r="J24" s="8" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
+    <row r="25" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
       <c r="D25" s="1" t="s">
         <v>43</v>
       </c>
@@ -2261,15 +2306,15 @@
       <c r="H25" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="I25" s="17"/>
+      <c r="I25" s="21"/>
       <c r="J25" s="8" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="24"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24" t="s">
+    <row r="26" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19" t="s">
         <v>45</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -2287,15 +2332,15 @@
       <c r="H26" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="I26" s="17"/>
+      <c r="I26" s="21"/>
       <c r="J26" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="24"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
+    <row r="27" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
       <c r="D27" s="1" t="s">
         <v>42</v>
       </c>
@@ -2311,15 +2356,15 @@
       <c r="H27" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="I27" s="17"/>
+      <c r="I27" s="21"/>
       <c r="J27" s="8" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="24"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
+    <row r="28" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
       <c r="D28" s="1" t="s">
         <v>43</v>
       </c>
@@ -2335,15 +2380,15 @@
       <c r="H28" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="I28" s="17"/>
+      <c r="I28" s="21"/>
       <c r="J28" s="8" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="24"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24" t="s">
+    <row r="29" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19" t="s">
         <v>46</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -2361,15 +2406,15 @@
       <c r="H29" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="I29" s="17"/>
+      <c r="I29" s="21"/>
       <c r="J29" s="8" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="24"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
+    <row r="30" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A30" s="19"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
       <c r="D30" s="1" t="s">
         <v>42</v>
       </c>
@@ -2385,28 +2430,28 @@
       <c r="H30" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="I30" s="17"/>
+      <c r="I30" s="21"/>
       <c r="J30" s="8" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="24"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
+    <row r="31" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
       <c r="D31" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="I31" s="17"/>
+      <c r="I31" s="21"/>
       <c r="J31" s="8"/>
     </row>
-    <row r="32" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="24"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="24" t="s">
+    <row r="32" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A32" s="19"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19" t="s">
         <v>47</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -2424,15 +2469,15 @@
       <c r="H32" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="I32" s="17"/>
+      <c r="I32" s="21"/>
       <c r="J32" s="8" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="24"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
+    <row r="33" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A33" s="19"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
       <c r="D33" s="1" t="s">
         <v>42</v>
       </c>
@@ -2448,15 +2493,15 @@
       <c r="H33" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="I33" s="17"/>
+      <c r="I33" s="21"/>
       <c r="J33" s="8" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="24"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
+    <row r="34" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A34" s="19"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
       <c r="D34" s="1" t="s">
         <v>43</v>
       </c>
@@ -2472,15 +2517,15 @@
       <c r="H34" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="I34" s="17"/>
+      <c r="I34" s="21"/>
       <c r="J34" s="8" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="24"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="24" t="s">
+    <row r="35" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A35" s="19"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19" t="s">
         <v>48</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -2498,15 +2543,15 @@
       <c r="H35" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="I35" s="17"/>
+      <c r="I35" s="21"/>
       <c r="J35" s="8" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="24"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
+    <row r="36" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A36" s="19"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
       <c r="D36" s="1" t="s">
         <v>42</v>
       </c>
@@ -2522,28 +2567,28 @@
       <c r="H36" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="I36" s="17"/>
+      <c r="I36" s="21"/>
       <c r="J36" s="8" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="24"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
+    <row r="37" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A37" s="19"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
       <c r="D37" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="I37" s="17"/>
+      <c r="I37" s="21"/>
       <c r="J37" s="8"/>
     </row>
-    <row r="38" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="24"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="24" t="s">
+    <row r="38" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A38" s="19"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19" t="s">
         <v>49</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -2561,15 +2606,15 @@
       <c r="H38" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="I38" s="17"/>
+      <c r="I38" s="21"/>
       <c r="J38" s="8" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="24"/>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
+    <row r="39" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A39" s="19"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
       <c r="D39" s="1" t="s">
         <v>42</v>
       </c>
@@ -2585,28 +2630,28 @@
       <c r="H39" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="I39" s="17"/>
+      <c r="I39" s="21"/>
       <c r="J39" s="8" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="24"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
+    <row r="40" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A40" s="19"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
       <c r="D40" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="I40" s="17"/>
+      <c r="I40" s="21"/>
       <c r="J40" s="8"/>
     </row>
-    <row r="41" spans="1:10" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="24"/>
-      <c r="B41" s="24"/>
-      <c r="C41" s="24" t="s">
+    <row r="41" spans="1:10" ht="58.5" customHeight="1">
+      <c r="A41" s="19"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19" t="s">
         <v>128</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -2624,15 +2669,15 @@
       <c r="H41" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="I41" s="17"/>
+      <c r="I41" s="21"/>
       <c r="J41" s="8" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="24"/>
-      <c r="B42" s="24"/>
-      <c r="C42" s="24"/>
+    <row r="42" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A42" s="19"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
       <c r="D42" s="1" t="s">
         <v>42</v>
       </c>
@@ -2648,15 +2693,15 @@
       <c r="H42" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="I42" s="17"/>
+      <c r="I42" s="21"/>
       <c r="J42" s="8" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="24"/>
-      <c r="B43" s="24"/>
-      <c r="C43" s="24"/>
+    <row r="43" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A43" s="19"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
       <c r="D43" s="1" t="s">
         <v>43</v>
       </c>
@@ -2672,15 +2717,15 @@
       <c r="H43" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="I43" s="17"/>
+      <c r="I43" s="21"/>
       <c r="J43" s="8" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="24"/>
-      <c r="B44" s="24"/>
-      <c r="C44" s="24" t="s">
+    <row r="44" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A44" s="19"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19" t="s">
         <v>50</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -2689,13 +2734,13 @@
       <c r="E44" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="I44" s="17"/>
+      <c r="I44" s="21"/>
       <c r="J44" s="8"/>
     </row>
-    <row r="45" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="24"/>
-      <c r="B45" s="24"/>
-      <c r="C45" s="24"/>
+    <row r="45" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A45" s="19"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
       <c r="D45" s="1" t="s">
         <v>42</v>
       </c>
@@ -2711,28 +2756,28 @@
       <c r="H45" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="I45" s="17"/>
+      <c r="I45" s="21"/>
       <c r="J45" s="8" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="24"/>
-      <c r="B46" s="24"/>
-      <c r="C46" s="24"/>
+    <row r="46" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A46" s="19"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
       <c r="D46" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="I46" s="17"/>
+      <c r="I46" s="21"/>
       <c r="J46" s="8"/>
     </row>
-    <row r="47" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="24"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="24" t="s">
+    <row r="47" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A47" s="19"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19" t="s">
         <v>51</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -2750,15 +2795,15 @@
       <c r="H47" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I47" s="17"/>
+      <c r="I47" s="21"/>
       <c r="J47" s="8" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="24"/>
-      <c r="B48" s="24"/>
-      <c r="C48" s="24"/>
+    <row r="48" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A48" s="19"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
       <c r="D48" s="1" t="s">
         <v>42</v>
       </c>
@@ -2774,15 +2819,15 @@
       <c r="H48" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="I48" s="17"/>
+      <c r="I48" s="21"/>
       <c r="J48" s="8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="24"/>
-      <c r="B49" s="24"/>
-      <c r="C49" s="24"/>
+    <row r="49" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A49" s="19"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="19"/>
       <c r="D49" s="1" t="s">
         <v>43</v>
       </c>
@@ -2798,15 +2843,15 @@
       <c r="H49" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="I49" s="17"/>
+      <c r="I49" s="21"/>
       <c r="J49" s="8" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="24"/>
-      <c r="B50" s="24"/>
-      <c r="C50" s="24" t="s">
+    <row r="50" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A50" s="19"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19" t="s">
         <v>52</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -2815,13 +2860,13 @@
       <c r="E50" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="I50" s="17"/>
+      <c r="I50" s="21"/>
       <c r="J50" s="8"/>
     </row>
-    <row r="51" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="24"/>
-      <c r="B51" s="24"/>
-      <c r="C51" s="24"/>
+    <row r="51" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A51" s="19"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="19"/>
       <c r="D51" s="1" t="s">
         <v>42</v>
       </c>
@@ -2834,15 +2879,15 @@
       <c r="H51" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="I51" s="17"/>
+      <c r="I51" s="21"/>
       <c r="J51" s="8" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="24"/>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
+    <row r="52" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A52" s="19"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="19"/>
       <c r="D52" s="1" t="s">
         <v>43</v>
       </c>
@@ -2855,15 +2900,15 @@
       <c r="H52" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="I52" s="17"/>
+      <c r="I52" s="21"/>
       <c r="J52" s="8" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="24"/>
-      <c r="B53" s="24"/>
-      <c r="C53" s="24" t="s">
+    <row r="53" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A53" s="19"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="19" t="s">
         <v>53</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -2872,13 +2917,13 @@
       <c r="E53" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="I53" s="17"/>
+      <c r="I53" s="21"/>
       <c r="J53" s="8"/>
     </row>
-    <row r="54" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="24"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="24"/>
+    <row r="54" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A54" s="19"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="19"/>
       <c r="D54" s="1" t="s">
         <v>42</v>
       </c>
@@ -2891,15 +2936,15 @@
       <c r="H54" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="I54" s="17"/>
+      <c r="I54" s="21"/>
       <c r="J54" s="8" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="23"/>
-      <c r="B55" s="23"/>
-      <c r="C55" s="23"/>
+    <row r="55" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A55" s="17"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="17"/>
       <c r="D55" s="3" t="s">
         <v>43</v>
       </c>
@@ -2913,22 +2958,22 @@
       <c r="H55" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="I55" s="18"/>
+      <c r="I55" s="22"/>
       <c r="J55" s="14" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="25">
+    <row r="56" spans="1:10" ht="66" customHeight="1">
+      <c r="A56" s="16">
         <v>7</v>
       </c>
-      <c r="B56" s="25" t="s">
+      <c r="B56" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="C56" s="25" t="s">
+      <c r="C56" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D56" s="25"/>
+      <c r="D56" s="16"/>
       <c r="E56" s="1" t="b">
         <v>1</v>
       </c>
@@ -2941,20 +2986,20 @@
       <c r="H56" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="I56" s="19" t="s">
+      <c r="I56" s="23" t="s">
         <v>212</v>
       </c>
       <c r="J56" s="8">
         <v>100000000</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="24"/>
-      <c r="B57" s="24"/>
-      <c r="C57" s="24" t="s">
+    <row r="57" spans="1:10" ht="66" customHeight="1">
+      <c r="A57" s="19"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="D57" s="24"/>
+      <c r="D57" s="19"/>
       <c r="E57" s="1" t="b">
         <v>1</v>
       </c>
@@ -2967,18 +3012,18 @@
       <c r="H57" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I57" s="20"/>
+      <c r="I57" s="24"/>
       <c r="J57" s="8">
         <v>4.4299999999999999E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="24"/>
-      <c r="B58" s="24"/>
-      <c r="C58" s="24" t="s">
+    <row r="58" spans="1:10" ht="66" customHeight="1">
+      <c r="A58" s="19"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="D58" s="24"/>
+      <c r="D58" s="19"/>
       <c r="E58" s="1" t="b">
         <v>1</v>
       </c>
@@ -2991,18 +3036,18 @@
       <c r="H58" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I58" s="20"/>
+      <c r="I58" s="24"/>
       <c r="J58" s="8">
         <v>300</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="24"/>
-      <c r="B59" s="24"/>
-      <c r="C59" s="24" t="s">
+    <row r="59" spans="1:10" ht="66" customHeight="1">
+      <c r="A59" s="19"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="D59" s="24"/>
+      <c r="D59" s="19"/>
       <c r="E59" s="1" t="b">
         <v>1</v>
       </c>
@@ -3015,18 +3060,18 @@
       <c r="H59" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I59" s="20"/>
+      <c r="I59" s="24"/>
       <c r="J59" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="24"/>
-      <c r="B60" s="24"/>
-      <c r="C60" s="24" t="s">
+    <row r="60" spans="1:10" ht="66" customHeight="1">
+      <c r="A60" s="19"/>
+      <c r="B60" s="19"/>
+      <c r="C60" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D60" s="24"/>
+      <c r="D60" s="19"/>
       <c r="E60" s="1" t="b">
         <v>1</v>
       </c>
@@ -3039,18 +3084,18 @@
       <c r="H60" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I60" s="20"/>
+      <c r="I60" s="24"/>
       <c r="J60" s="8">
         <v>100000000</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="24"/>
-      <c r="B61" s="24"/>
-      <c r="C61" s="24" t="s">
+    <row r="61" spans="1:10" ht="66" customHeight="1">
+      <c r="A61" s="19"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="D61" s="24"/>
+      <c r="D61" s="19"/>
       <c r="E61" s="1" t="b">
         <v>1</v>
       </c>
@@ -3063,18 +3108,18 @@
       <c r="H61" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I61" s="20"/>
+      <c r="I61" s="24"/>
       <c r="J61" s="8">
         <v>6.6199999999999995E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="24"/>
-      <c r="B62" s="24"/>
-      <c r="C62" s="24" t="s">
+    <row r="62" spans="1:10" ht="66" customHeight="1">
+      <c r="A62" s="19"/>
+      <c r="B62" s="19"/>
+      <c r="C62" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="D62" s="24"/>
+      <c r="D62" s="19"/>
       <c r="E62" s="1" t="b">
         <v>1</v>
       </c>
@@ -3087,18 +3132,18 @@
       <c r="H62" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I62" s="20"/>
+      <c r="I62" s="24"/>
       <c r="J62" s="8">
         <v>120</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="24"/>
-      <c r="B63" s="24"/>
-      <c r="C63" s="24" t="s">
+    <row r="63" spans="1:10" ht="66" customHeight="1">
+      <c r="A63" s="19"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="D63" s="24"/>
+      <c r="D63" s="19"/>
       <c r="E63" s="1" t="b">
         <v>1</v>
       </c>
@@ -3111,18 +3156,18 @@
       <c r="H63" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I63" s="20"/>
+      <c r="I63" s="24"/>
       <c r="J63" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="24"/>
-      <c r="B64" s="24"/>
-      <c r="C64" s="24" t="s">
+    <row r="64" spans="1:10" ht="66" customHeight="1">
+      <c r="A64" s="19"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="D64" s="24"/>
+      <c r="D64" s="19"/>
       <c r="E64" s="1" t="b">
         <v>1</v>
       </c>
@@ -3135,18 +3180,18 @@
       <c r="H64" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="I64" s="20"/>
+      <c r="I64" s="24"/>
       <c r="J64" s="8" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="24"/>
-      <c r="B65" s="24"/>
-      <c r="C65" s="24" t="s">
+    <row r="65" spans="1:10" ht="66" customHeight="1">
+      <c r="A65" s="19"/>
+      <c r="B65" s="19"/>
+      <c r="C65" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="D65" s="24"/>
+      <c r="D65" s="19"/>
       <c r="E65" s="1" t="b">
         <v>1</v>
       </c>
@@ -3159,18 +3204,18 @@
       <c r="H65" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="I65" s="20"/>
+      <c r="I65" s="24"/>
       <c r="J65" s="8" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="24"/>
-      <c r="B66" s="24"/>
-      <c r="C66" s="24" t="s">
+    <row r="66" spans="1:10" ht="66" customHeight="1">
+      <c r="A66" s="19"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="D66" s="24"/>
+      <c r="D66" s="19"/>
       <c r="E66" s="1" t="b">
         <v>1</v>
       </c>
@@ -3183,18 +3228,18 @@
       <c r="H66" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="I66" s="20"/>
+      <c r="I66" s="24"/>
       <c r="J66" s="8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="24"/>
-      <c r="B67" s="24"/>
-      <c r="C67" s="24" t="s">
+    <row r="67" spans="1:10" ht="66" customHeight="1">
+      <c r="A67" s="19"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="D67" s="24"/>
+      <c r="D67" s="19"/>
       <c r="E67" s="1" t="b">
         <v>1</v>
       </c>
@@ -3207,18 +3252,18 @@
       <c r="H67" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="I67" s="20"/>
+      <c r="I67" s="24"/>
       <c r="J67" s="8" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="24"/>
-      <c r="B68" s="24"/>
-      <c r="C68" s="24" t="s">
+    <row r="68" spans="1:10" ht="66" customHeight="1">
+      <c r="A68" s="19"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="D68" s="24"/>
+      <c r="D68" s="19"/>
       <c r="E68" s="1" t="b">
         <v>1</v>
       </c>
@@ -3231,18 +3276,18 @@
       <c r="H68" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="I68" s="20"/>
+      <c r="I68" s="24"/>
       <c r="J68" s="8" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="23"/>
-      <c r="B69" s="23"/>
-      <c r="C69" s="23" t="s">
+    <row r="69" spans="1:10" ht="66" customHeight="1">
+      <c r="A69" s="17"/>
+      <c r="B69" s="17"/>
+      <c r="C69" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D69" s="23"/>
+      <c r="D69" s="17"/>
       <c r="E69" s="3" t="b">
         <v>1</v>
       </c>
@@ -3255,214 +3300,230 @@
       <c r="H69" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="I69" s="21"/>
+      <c r="I69" s="25"/>
       <c r="J69" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="71" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="73" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="78" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="79" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="81" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="82" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="83" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="85" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="86" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="87" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="88" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="89" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="90" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="91" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="92" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="93" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="94" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="95" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="96" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="97" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="98" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="99" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="100" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="101" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="102" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="103" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="104" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="105" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="106" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="107" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="108" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="109" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="110" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="111" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="112" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="113" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="114" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="115" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="116" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="117" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="118" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="119" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="120" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="121" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="122" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="123" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="124" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="125" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="126" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="127" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="128" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="129" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="130" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="131" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="132" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="133" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="134" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="135" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="136" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="137" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="138" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="139" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="140" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="141" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="142" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="143" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="144" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="145" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="146" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="147" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="148" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="149" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="150" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="151" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="152" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="153" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="154" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="155" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="156" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="157" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="158" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="159" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="160" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="161" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="162" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="163" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="164" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="165" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="166" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="167" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="168" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="169" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="170" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="171" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="172" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="173" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="174" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="175" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="176" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="177" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="178" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="179" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="180" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="181" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="182" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="183" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="184" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="185" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="186" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="187" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="188" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="189" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="190" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="191" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="192" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="193" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="194" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="195" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="196" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="197" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="198" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="199" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="200" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="201" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="202" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="203" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="204" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="205" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="206" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="207" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="208" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="209" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="210" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="211" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="212" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="213" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="214" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="215" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="216" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="217" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="218" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="219" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="220" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="221" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="222" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="223" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="224" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="225" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="226" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="227" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="228" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="229" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="230" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="231" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="232" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="233" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="234" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="235" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="236" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="237" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="238" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="239" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="240" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="241" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="242" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="243" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="244" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="245" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="246" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="247" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="248" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="249" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="250" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="251" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="252" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="253" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="254" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="255" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" spans="1:10" ht="32.25" customHeight="1"/>
+    <row r="71" spans="1:10" ht="32.25" customHeight="1"/>
+    <row r="72" spans="1:10" ht="32.25" customHeight="1"/>
+    <row r="73" spans="1:10" ht="32.25" customHeight="1"/>
+    <row r="74" spans="1:10" ht="32.25" customHeight="1"/>
+    <row r="75" spans="1:10" ht="32.25" customHeight="1"/>
+    <row r="76" spans="1:10" ht="32.25" customHeight="1"/>
+    <row r="77" spans="1:10" ht="32.25" customHeight="1"/>
+    <row r="78" spans="1:10" ht="32.25" customHeight="1"/>
+    <row r="79" spans="1:10" ht="32.25" customHeight="1"/>
+    <row r="80" spans="1:10" ht="32.25" customHeight="1"/>
+    <row r="81" ht="32.25" customHeight="1"/>
+    <row r="82" ht="32.25" customHeight="1"/>
+    <row r="83" ht="32.25" customHeight="1"/>
+    <row r="84" ht="32.25" customHeight="1"/>
+    <row r="85" ht="32.25" customHeight="1"/>
+    <row r="86" ht="32.25" customHeight="1"/>
+    <row r="87" ht="32.25" customHeight="1"/>
+    <row r="88" ht="32.25" customHeight="1"/>
+    <row r="89" ht="32.25" customHeight="1"/>
+    <row r="90" ht="32.25" customHeight="1"/>
+    <row r="91" ht="32.25" customHeight="1"/>
+    <row r="92" ht="32.25" customHeight="1"/>
+    <row r="93" ht="32.25" customHeight="1"/>
+    <row r="94" ht="32.25" customHeight="1"/>
+    <row r="95" ht="32.25" customHeight="1"/>
+    <row r="96" ht="32.25" customHeight="1"/>
+    <row r="97" ht="32.25" customHeight="1"/>
+    <row r="98" ht="32.25" customHeight="1"/>
+    <row r="99" ht="32.25" customHeight="1"/>
+    <row r="100" ht="32.25" customHeight="1"/>
+    <row r="101" ht="32.25" customHeight="1"/>
+    <row r="102" ht="32.25" customHeight="1"/>
+    <row r="103" ht="32.25" customHeight="1"/>
+    <row r="104" ht="32.25" customHeight="1"/>
+    <row r="105" ht="32.25" customHeight="1"/>
+    <row r="106" ht="32.25" customHeight="1"/>
+    <row r="107" ht="32.25" customHeight="1"/>
+    <row r="108" ht="32.25" customHeight="1"/>
+    <row r="109" ht="32.25" customHeight="1"/>
+    <row r="110" ht="32.25" customHeight="1"/>
+    <row r="111" ht="32.25" customHeight="1"/>
+    <row r="112" ht="32.25" customHeight="1"/>
+    <row r="113" ht="32.25" customHeight="1"/>
+    <row r="114" ht="32.25" customHeight="1"/>
+    <row r="115" ht="32.25" customHeight="1"/>
+    <row r="116" ht="32.25" customHeight="1"/>
+    <row r="117" ht="32.25" customHeight="1"/>
+    <row r="118" ht="32.25" customHeight="1"/>
+    <row r="119" ht="32.25" customHeight="1"/>
+    <row r="120" ht="32.25" customHeight="1"/>
+    <row r="121" ht="32.25" customHeight="1"/>
+    <row r="122" ht="32.25" customHeight="1"/>
+    <row r="123" ht="32.25" customHeight="1"/>
+    <row r="124" ht="32.25" customHeight="1"/>
+    <row r="125" ht="32.25" customHeight="1"/>
+    <row r="126" ht="32.25" customHeight="1"/>
+    <row r="127" ht="32.25" customHeight="1"/>
+    <row r="128" ht="32.25" customHeight="1"/>
+    <row r="129" ht="32.25" customHeight="1"/>
+    <row r="130" ht="32.25" customHeight="1"/>
+    <row r="131" ht="32.25" customHeight="1"/>
+    <row r="132" ht="32.25" customHeight="1"/>
+    <row r="133" ht="32.25" customHeight="1"/>
+    <row r="134" ht="32.25" customHeight="1"/>
+    <row r="135" ht="32.25" customHeight="1"/>
+    <row r="136" ht="32.25" customHeight="1"/>
+    <row r="137" ht="32.25" customHeight="1"/>
+    <row r="138" ht="32.25" customHeight="1"/>
+    <row r="139" ht="32.25" customHeight="1"/>
+    <row r="140" ht="32.25" customHeight="1"/>
+    <row r="141" ht="32.25" customHeight="1"/>
+    <row r="142" ht="32.25" customHeight="1"/>
+    <row r="143" ht="32.25" customHeight="1"/>
+    <row r="144" ht="32.25" customHeight="1"/>
+    <row r="145" ht="32.25" customHeight="1"/>
+    <row r="146" ht="32.25" customHeight="1"/>
+    <row r="147" ht="32.25" customHeight="1"/>
+    <row r="148" ht="32.25" customHeight="1"/>
+    <row r="149" ht="32.25" customHeight="1"/>
+    <row r="150" ht="32.25" customHeight="1"/>
+    <row r="151" ht="32.25" customHeight="1"/>
+    <row r="152" ht="32.25" customHeight="1"/>
+    <row r="153" ht="32.25" customHeight="1"/>
+    <row r="154" ht="32.25" customHeight="1"/>
+    <row r="155" ht="32.25" customHeight="1"/>
+    <row r="156" ht="32.25" customHeight="1"/>
+    <row r="157" ht="32.25" customHeight="1"/>
+    <row r="158" ht="32.25" customHeight="1"/>
+    <row r="159" ht="32.25" customHeight="1"/>
+    <row r="160" ht="32.25" customHeight="1"/>
+    <row r="161" ht="32.25" customHeight="1"/>
+    <row r="162" ht="32.25" customHeight="1"/>
+    <row r="163" ht="32.25" customHeight="1"/>
+    <row r="164" ht="32.25" customHeight="1"/>
+    <row r="165" ht="32.25" customHeight="1"/>
+    <row r="166" ht="32.25" customHeight="1"/>
+    <row r="167" ht="32.25" customHeight="1"/>
+    <row r="168" ht="32.25" customHeight="1"/>
+    <row r="169" ht="32.25" customHeight="1"/>
+    <row r="170" ht="32.25" customHeight="1"/>
+    <row r="171" ht="32.25" customHeight="1"/>
+    <row r="172" ht="32.25" customHeight="1"/>
+    <row r="173" ht="32.25" customHeight="1"/>
+    <row r="174" ht="32.25" customHeight="1"/>
+    <row r="175" ht="32.25" customHeight="1"/>
+    <row r="176" ht="32.25" customHeight="1"/>
+    <row r="177" ht="32.25" customHeight="1"/>
+    <row r="178" ht="32.25" customHeight="1"/>
+    <row r="179" ht="32.25" customHeight="1"/>
+    <row r="180" ht="32.25" customHeight="1"/>
+    <row r="181" ht="32.25" customHeight="1"/>
+    <row r="182" ht="32.25" customHeight="1"/>
+    <row r="183" ht="32.25" customHeight="1"/>
+    <row r="184" ht="32.25" customHeight="1"/>
+    <row r="185" ht="32.25" customHeight="1"/>
+    <row r="186" ht="32.25" customHeight="1"/>
+    <row r="187" ht="32.25" customHeight="1"/>
+    <row r="188" ht="32.25" customHeight="1"/>
+    <row r="189" ht="32.25" customHeight="1"/>
+    <row r="190" ht="32.25" customHeight="1"/>
+    <row r="191" ht="32.25" customHeight="1"/>
+    <row r="192" ht="32.25" customHeight="1"/>
+    <row r="193" ht="32.25" customHeight="1"/>
+    <row r="194" ht="32.25" customHeight="1"/>
+    <row r="195" ht="32.25" customHeight="1"/>
+    <row r="196" ht="32.25" customHeight="1"/>
+    <row r="197" ht="32.25" customHeight="1"/>
+    <row r="198" ht="32.25" customHeight="1"/>
+    <row r="199" ht="32.25" customHeight="1"/>
+    <row r="200" ht="32.25" customHeight="1"/>
+    <row r="201" ht="32.25" customHeight="1"/>
+    <row r="202" ht="32.25" customHeight="1"/>
+    <row r="203" ht="32.25" customHeight="1"/>
+    <row r="204" ht="32.25" customHeight="1"/>
+    <row r="205" ht="32.25" customHeight="1"/>
+    <row r="206" ht="32.25" customHeight="1"/>
+    <row r="207" ht="32.25" customHeight="1"/>
+    <row r="208" ht="32.25" customHeight="1"/>
+    <row r="209" ht="32.25" customHeight="1"/>
+    <row r="210" ht="32.25" customHeight="1"/>
+    <row r="211" ht="32.25" customHeight="1"/>
+    <row r="212" ht="32.25" customHeight="1"/>
+    <row r="213" ht="32.25" customHeight="1"/>
+    <row r="214" ht="32.25" customHeight="1"/>
+    <row r="215" ht="32.25" customHeight="1"/>
+    <row r="216" ht="32.25" customHeight="1"/>
+    <row r="217" ht="32.25" customHeight="1"/>
+    <row r="218" ht="32.25" customHeight="1"/>
+    <row r="219" ht="32.25" customHeight="1"/>
+    <row r="220" ht="32.25" customHeight="1"/>
+    <row r="221" ht="32.25" customHeight="1"/>
+    <row r="222" ht="32.25" customHeight="1"/>
+    <row r="223" ht="32.25" customHeight="1"/>
+    <row r="224" ht="32.25" customHeight="1"/>
+    <row r="225" ht="32.25" customHeight="1"/>
+    <row r="226" ht="32.25" customHeight="1"/>
+    <row r="227" ht="32.25" customHeight="1"/>
+    <row r="228" ht="32.25" customHeight="1"/>
+    <row r="229" ht="32.25" customHeight="1"/>
+    <row r="230" ht="32.25" customHeight="1"/>
+    <row r="231" ht="32.25" customHeight="1"/>
+    <row r="232" ht="32.25" customHeight="1"/>
+    <row r="233" ht="32.25" customHeight="1"/>
+    <row r="234" ht="32.25" customHeight="1"/>
+    <row r="235" ht="32.25" customHeight="1"/>
+    <row r="236" ht="32.25" customHeight="1"/>
+    <row r="237" ht="32.25" customHeight="1"/>
+    <row r="238" ht="32.25" customHeight="1"/>
+    <row r="239" ht="32.25" customHeight="1"/>
+    <row r="240" ht="32.25" customHeight="1"/>
+    <row r="241" ht="32.25" customHeight="1"/>
+    <row r="242" ht="32.25" customHeight="1"/>
+    <row r="243" ht="32.25" customHeight="1"/>
+    <row r="244" ht="32.25" customHeight="1"/>
+    <row r="245" ht="32.25" customHeight="1"/>
+    <row r="246" ht="32.25" customHeight="1"/>
+    <row r="247" ht="32.25" customHeight="1"/>
+    <row r="248" ht="32.25" customHeight="1"/>
+    <row r="249" ht="32.25" customHeight="1"/>
+    <row r="250" ht="32.25" customHeight="1"/>
+    <row r="251" ht="32.25" customHeight="1"/>
+    <row r="252" ht="32.25" customHeight="1"/>
+    <row r="253" ht="32.25" customHeight="1"/>
+    <row r="254" ht="32.25" customHeight="1"/>
+    <row r="255" ht="32.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="I17:I55"/>
+    <mergeCell ref="I56:I69"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="B56:B69"/>
+    <mergeCell ref="A56:A69"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
     <mergeCell ref="B17:B55"/>
     <mergeCell ref="A17:A55"/>
     <mergeCell ref="C4:D4"/>
@@ -3479,38 +3540,22 @@
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="C20:C22"/>
     <mergeCell ref="C23:C25"/>
-    <mergeCell ref="B56:B69"/>
-    <mergeCell ref="A56:A69"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A11:A12"/>
     <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="I17:I55"/>
-    <mergeCell ref="I56:I69"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3518,14 +3563,216 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0B83C18-EA6E-4169-B9B4-45A14A2F7B14}">
+  <dimension ref="A6:M24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="2" max="4" width="16.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="1:4">
+      <c r="C6" t="s">
+        <v>253</v>
+      </c>
+      <c r="D6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C7" t="s">
+        <v>252</v>
+      </c>
+      <c r="D7" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>2022</v>
+      </c>
+      <c r="C9">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D9">
+        <v>4.92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>2021</v>
+      </c>
+      <c r="C10">
+        <v>2.5</v>
+      </c>
+      <c r="D10">
+        <v>3.04</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>2020</v>
+      </c>
+      <c r="C11">
+        <v>0.5</v>
+      </c>
+      <c r="D11">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>2019</v>
+      </c>
+      <c r="C12">
+        <v>0.4</v>
+      </c>
+      <c r="D12">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>2018</v>
+      </c>
+      <c r="C13">
+        <v>1.5</v>
+      </c>
+      <c r="D13">
+        <v>3.71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>2017</v>
+      </c>
+      <c r="C14">
+        <v>1.9</v>
+      </c>
+      <c r="D14">
+        <v>3.48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>2016</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>2015</v>
+      </c>
+      <c r="C16">
+        <v>0.7</v>
+      </c>
+      <c r="D16">
+        <v>3.54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17">
+        <v>2014</v>
+      </c>
+      <c r="C17">
+        <v>1.3</v>
+      </c>
+      <c r="D17">
+        <v>4.21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18">
+        <v>2013</v>
+      </c>
+      <c r="C18">
+        <v>1.3</v>
+      </c>
+      <c r="D18">
+        <v>4.72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19">
+        <v>2012</v>
+      </c>
+      <c r="C19">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D19">
+        <v>5.31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="17.25" thickBot="1">
+      <c r="B24" s="27">
+        <v>0.6</v>
+      </c>
+      <c r="C24" s="27">
+        <v>1.5</v>
+      </c>
+      <c r="D24" s="27">
+        <v>4.3</v>
+      </c>
+      <c r="E24" s="27">
+        <v>3.2</v>
+      </c>
+      <c r="F24" s="27">
+        <v>1.2</v>
+      </c>
+      <c r="G24" s="27">
+        <v>1.4</v>
+      </c>
+      <c r="H24" s="27">
+        <v>0.3</v>
+      </c>
+      <c r="I24" s="27">
+        <v>3.3</v>
+      </c>
+      <c r="J24" s="27">
+        <v>3.6</v>
+      </c>
+      <c r="K24" s="27">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="L24" s="27">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="M24" s="27">
+        <v>2.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84B899BD-BE4A-4CC0-811C-81D0F0532537}">
   <dimension ref="A1:G204"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="A4:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="4.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="1" customWidth="1"/>
@@ -3537,15 +3784,15 @@
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="26"/>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="31.5" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -3568,11 +3815,11 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="24">
-        <v>1</v>
-      </c>
-      <c r="B4" s="25" t="s">
+    <row r="4" spans="1:7" ht="32.25" customHeight="1">
+      <c r="A4" s="19">
+        <v>1</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>204</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -3584,16 +3831,16 @@
       <c r="E4" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="23" t="s">
         <v>246</v>
       </c>
       <c r="G4" s="1">
         <v>20000000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
+    <row r="5" spans="1:7" ht="32.25" customHeight="1">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="1" t="s">
         <v>214</v>
       </c>
@@ -3603,14 +3850,14 @@
       <c r="E5" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="F5" s="20"/>
+      <c r="F5" s="24"/>
       <c r="G5" s="1">
         <v>60000000</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
+    <row r="6" spans="1:7" ht="32.25" customHeight="1">
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="1" t="s">
         <v>215</v>
       </c>
@@ -3620,14 +3867,14 @@
       <c r="E6" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="F6" s="20"/>
+      <c r="F6" s="24"/>
       <c r="G6" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
+    <row r="7" spans="1:7" ht="32.25" customHeight="1">
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="1" t="s">
         <v>216</v>
       </c>
@@ -3637,14 +3884,14 @@
       <c r="E7" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="F7" s="20"/>
+      <c r="F7" s="24"/>
       <c r="G7" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="24"/>
-      <c r="B8" s="24"/>
+    <row r="8" spans="1:7" ht="32.25" customHeight="1">
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="1" t="s">
         <v>217</v>
       </c>
@@ -3654,14 +3901,14 @@
       <c r="E8" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="F8" s="20"/>
+      <c r="F8" s="24"/>
       <c r="G8" s="1">
         <v>86762000</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
+    <row r="9" spans="1:7" ht="32.25" customHeight="1">
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="1" t="s">
         <v>218</v>
       </c>
@@ -3671,11 +3918,11 @@
       <c r="E9" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="F9" s="20"/>
-    </row>
-    <row r="10" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="24"/>
-      <c r="B10" s="24"/>
+      <c r="F9" s="24"/>
+    </row>
+    <row r="10" spans="1:7" ht="32.25" customHeight="1">
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="1" t="s">
         <v>219</v>
       </c>
@@ -3685,9 +3932,9 @@
       <c r="E10" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="F10" s="20"/>
-    </row>
-    <row r="11" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="24"/>
+    </row>
+    <row r="11" spans="1:7" ht="32.25" customHeight="1">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -3704,7 +3951,7 @@
         <v>0.11993139923963493</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="32.25" customHeight="1">
       <c r="A12" s="1">
         <v>3</v>
       </c>
@@ -3721,7 +3968,7 @@
         <v>0.35979419771890481</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="32.25" customHeight="1">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -3738,7 +3985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="32.25" customHeight="1">
       <c r="A14" s="1">
         <v>5</v>
       </c>
@@ -3755,7 +4002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="32.25" customHeight="1">
       <c r="A15" s="1">
         <v>6</v>
       </c>
@@ -3772,7 +4019,7 @@
         <v>0.52027440304146033</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="32.25" customHeight="1">
       <c r="A16" s="1">
         <v>7</v>
       </c>
@@ -3789,7 +4036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="32.25" customHeight="1">
       <c r="A17" s="1">
         <v>8</v>
       </c>
@@ -3806,7 +4053,7 @@
         <v>166762000</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="32.25" customHeight="1">
       <c r="A18" s="1">
         <v>9</v>
       </c>
@@ -3823,7 +4070,7 @@
         <v>33293000</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="32.25" customHeight="1">
       <c r="A19" s="1">
         <v>10</v>
       </c>
@@ -3840,7 +4087,7 @@
         <v>1.1084847714660899</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="32.25" customHeight="1">
       <c r="A20" s="1">
         <v>11</v>
       </c>
@@ -3857,7 +4104,7 @@
         <v>-197417000</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="32.25" customHeight="1">
       <c r="A21" s="1">
         <v>12</v>
       </c>
@@ -3874,7 +4121,7 @@
         <v>340184000</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="32.25" customHeight="1">
       <c r="A22" s="1">
         <v>13</v>
       </c>
@@ -3891,7 +4138,7 @@
         <v>35873000</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="32.25" customHeight="1">
       <c r="A23" s="1">
         <v>14</v>
       </c>
@@ -3908,7 +4155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="32.25" customHeight="1">
       <c r="A24" s="1">
         <v>15</v>
       </c>
@@ -3925,7 +4172,7 @@
         <v>7665000</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="32.25" customHeight="1">
       <c r="A25" s="1">
         <v>16</v>
       </c>
@@ -3942,7 +4189,7 @@
         <v>9815000</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="32.25" customHeight="1">
       <c r="A26" s="1">
         <v>17</v>
       </c>
@@ -3959,7 +4206,7 @@
         <v>1808000</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="32.25" customHeight="1">
       <c r="A27" s="1">
         <v>18</v>
       </c>
@@ -3976,7 +4223,7 @@
         <v>754000</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="32.25" customHeight="1">
       <c r="A28" s="1">
         <v>19</v>
       </c>
@@ -3993,7 +4240,7 @@
         <v>9729000</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="32.25" customHeight="1">
       <c r="A29" s="1">
         <v>20</v>
       </c>
@@ -4010,7 +4257,7 @@
         <v>4063000</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="32.25" customHeight="1">
       <c r="A30" s="1">
         <v>21</v>
       </c>
@@ -4027,7 +4274,7 @@
         <v>1883000</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="32.25" customHeight="1">
       <c r="A31" s="1">
         <v>22</v>
       </c>
@@ -4044,7 +4291,7 @@
         <v>88889000</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="32.25" customHeight="1">
       <c r="A32" s="1">
         <v>23</v>
       </c>
@@ -4061,7 +4308,7 @@
         <v>760000</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="32.25" customHeight="1">
       <c r="A33" s="1">
         <v>24</v>
       </c>
@@ -4078,7 +4325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="32.25" customHeight="1">
       <c r="A34" s="1">
         <v>25</v>
       </c>
@@ -4095,180 +4342,180 @@
         <v>5523000</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="32.25" customHeight="1">
       <c r="A35" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="57" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="60" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="62" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="65" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="68" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="70" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="71" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="73" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="78" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="79" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="81" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="82" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="83" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="85" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="86" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="87" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="88" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="89" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="90" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="91" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="92" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="93" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="94" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="95" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="96" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="97" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="98" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="99" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="100" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="101" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="102" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="103" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="104" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="105" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="106" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="107" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="108" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="109" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="110" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="111" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="112" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="113" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="114" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="115" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="116" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="117" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="118" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="119" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="120" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="121" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="122" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="123" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="124" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="125" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="126" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="127" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="128" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="129" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="130" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="131" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="132" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="133" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="134" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="135" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="136" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="137" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="138" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="139" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="140" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="141" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="142" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="143" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="144" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="145" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="146" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="147" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="148" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="149" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="150" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="151" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="152" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="153" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="154" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="155" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="156" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="157" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="158" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="159" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="160" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="161" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="162" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="163" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="164" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="165" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="166" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="167" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="168" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="169" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="170" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="171" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="172" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="173" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="174" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="175" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="176" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="177" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="178" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="179" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="180" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="181" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="182" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="183" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="184" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="185" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="186" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="187" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="188" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="189" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="190" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="191" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="192" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="193" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="194" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="195" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="196" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="197" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="198" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="199" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="200" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="201" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="202" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="203" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="204" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:6" ht="32.25" customHeight="1"/>
+    <row r="37" spans="1:6" ht="32.25" customHeight="1"/>
+    <row r="38" spans="1:6" ht="32.25" customHeight="1"/>
+    <row r="39" spans="1:6" ht="32.25" customHeight="1"/>
+    <row r="40" spans="1:6" ht="32.25" customHeight="1"/>
+    <row r="41" spans="1:6" ht="32.25" customHeight="1"/>
+    <row r="42" spans="1:6" ht="32.25" customHeight="1"/>
+    <row r="43" spans="1:6" ht="32.25" customHeight="1"/>
+    <row r="44" spans="1:6" ht="32.25" customHeight="1"/>
+    <row r="45" spans="1:6" ht="32.25" customHeight="1"/>
+    <row r="46" spans="1:6" ht="32.25" customHeight="1"/>
+    <row r="47" spans="1:6" ht="32.25" customHeight="1"/>
+    <row r="48" spans="1:6" ht="32.25" customHeight="1"/>
+    <row r="49" ht="32.25" customHeight="1"/>
+    <row r="50" ht="32.25" customHeight="1"/>
+    <row r="51" ht="32.25" customHeight="1"/>
+    <row r="52" ht="32.25" customHeight="1"/>
+    <row r="53" ht="32.25" customHeight="1"/>
+    <row r="54" ht="32.25" customHeight="1"/>
+    <row r="55" ht="32.25" customHeight="1"/>
+    <row r="56" ht="32.25" customHeight="1"/>
+    <row r="57" ht="32.25" customHeight="1"/>
+    <row r="58" ht="32.25" customHeight="1"/>
+    <row r="59" ht="32.25" customHeight="1"/>
+    <row r="60" ht="32.25" customHeight="1"/>
+    <row r="61" ht="32.25" customHeight="1"/>
+    <row r="62" ht="32.25" customHeight="1"/>
+    <row r="63" ht="32.25" customHeight="1"/>
+    <row r="64" ht="32.25" customHeight="1"/>
+    <row r="65" ht="32.25" customHeight="1"/>
+    <row r="66" ht="32.25" customHeight="1"/>
+    <row r="67" ht="32.25" customHeight="1"/>
+    <row r="68" ht="32.25" customHeight="1"/>
+    <row r="69" ht="32.25" customHeight="1"/>
+    <row r="70" ht="32.25" customHeight="1"/>
+    <row r="71" ht="32.25" customHeight="1"/>
+    <row r="72" ht="32.25" customHeight="1"/>
+    <row r="73" ht="32.25" customHeight="1"/>
+    <row r="74" ht="32.25" customHeight="1"/>
+    <row r="75" ht="32.25" customHeight="1"/>
+    <row r="76" ht="32.25" customHeight="1"/>
+    <row r="77" ht="32.25" customHeight="1"/>
+    <row r="78" ht="32.25" customHeight="1"/>
+    <row r="79" ht="32.25" customHeight="1"/>
+    <row r="80" ht="32.25" customHeight="1"/>
+    <row r="81" ht="32.25" customHeight="1"/>
+    <row r="82" ht="32.25" customHeight="1"/>
+    <row r="83" ht="32.25" customHeight="1"/>
+    <row r="84" ht="32.25" customHeight="1"/>
+    <row r="85" ht="32.25" customHeight="1"/>
+    <row r="86" ht="32.25" customHeight="1"/>
+    <row r="87" ht="32.25" customHeight="1"/>
+    <row r="88" ht="32.25" customHeight="1"/>
+    <row r="89" ht="32.25" customHeight="1"/>
+    <row r="90" ht="32.25" customHeight="1"/>
+    <row r="91" ht="32.25" customHeight="1"/>
+    <row r="92" ht="32.25" customHeight="1"/>
+    <row r="93" ht="32.25" customHeight="1"/>
+    <row r="94" ht="32.25" customHeight="1"/>
+    <row r="95" ht="32.25" customHeight="1"/>
+    <row r="96" ht="32.25" customHeight="1"/>
+    <row r="97" ht="32.25" customHeight="1"/>
+    <row r="98" ht="32.25" customHeight="1"/>
+    <row r="99" ht="32.25" customHeight="1"/>
+    <row r="100" ht="32.25" customHeight="1"/>
+    <row r="101" ht="32.25" customHeight="1"/>
+    <row r="102" ht="32.25" customHeight="1"/>
+    <row r="103" ht="32.25" customHeight="1"/>
+    <row r="104" ht="32.25" customHeight="1"/>
+    <row r="105" ht="32.25" customHeight="1"/>
+    <row r="106" ht="32.25" customHeight="1"/>
+    <row r="107" ht="32.25" customHeight="1"/>
+    <row r="108" ht="32.25" customHeight="1"/>
+    <row r="109" ht="32.25" customHeight="1"/>
+    <row r="110" ht="32.25" customHeight="1"/>
+    <row r="111" ht="32.25" customHeight="1"/>
+    <row r="112" ht="32.25" customHeight="1"/>
+    <row r="113" ht="32.25" customHeight="1"/>
+    <row r="114" ht="32.25" customHeight="1"/>
+    <row r="115" ht="32.25" customHeight="1"/>
+    <row r="116" ht="32.25" customHeight="1"/>
+    <row r="117" ht="32.25" customHeight="1"/>
+    <row r="118" ht="32.25" customHeight="1"/>
+    <row r="119" ht="32.25" customHeight="1"/>
+    <row r="120" ht="32.25" customHeight="1"/>
+    <row r="121" ht="32.25" customHeight="1"/>
+    <row r="122" ht="32.25" customHeight="1"/>
+    <row r="123" ht="32.25" customHeight="1"/>
+    <row r="124" ht="32.25" customHeight="1"/>
+    <row r="125" ht="32.25" customHeight="1"/>
+    <row r="126" ht="32.25" customHeight="1"/>
+    <row r="127" ht="32.25" customHeight="1"/>
+    <row r="128" ht="32.25" customHeight="1"/>
+    <row r="129" ht="32.25" customHeight="1"/>
+    <row r="130" ht="32.25" customHeight="1"/>
+    <row r="131" ht="32.25" customHeight="1"/>
+    <row r="132" ht="32.25" customHeight="1"/>
+    <row r="133" ht="32.25" customHeight="1"/>
+    <row r="134" ht="32.25" customHeight="1"/>
+    <row r="135" ht="32.25" customHeight="1"/>
+    <row r="136" ht="32.25" customHeight="1"/>
+    <row r="137" ht="32.25" customHeight="1"/>
+    <row r="138" ht="32.25" customHeight="1"/>
+    <row r="139" ht="32.25" customHeight="1"/>
+    <row r="140" ht="32.25" customHeight="1"/>
+    <row r="141" ht="32.25" customHeight="1"/>
+    <row r="142" ht="32.25" customHeight="1"/>
+    <row r="143" ht="32.25" customHeight="1"/>
+    <row r="144" ht="32.25" customHeight="1"/>
+    <row r="145" ht="32.25" customHeight="1"/>
+    <row r="146" ht="32.25" customHeight="1"/>
+    <row r="147" ht="32.25" customHeight="1"/>
+    <row r="148" ht="32.25" customHeight="1"/>
+    <row r="149" ht="32.25" customHeight="1"/>
+    <row r="150" ht="32.25" customHeight="1"/>
+    <row r="151" ht="32.25" customHeight="1"/>
+    <row r="152" ht="32.25" customHeight="1"/>
+    <row r="153" ht="32.25" customHeight="1"/>
+    <row r="154" ht="32.25" customHeight="1"/>
+    <row r="155" ht="32.25" customHeight="1"/>
+    <row r="156" ht="32.25" customHeight="1"/>
+    <row r="157" ht="32.25" customHeight="1"/>
+    <row r="158" ht="32.25" customHeight="1"/>
+    <row r="159" ht="32.25" customHeight="1"/>
+    <row r="160" ht="32.25" customHeight="1"/>
+    <row r="161" ht="32.25" customHeight="1"/>
+    <row r="162" ht="32.25" customHeight="1"/>
+    <row r="163" ht="32.25" customHeight="1"/>
+    <row r="164" ht="32.25" customHeight="1"/>
+    <row r="165" ht="32.25" customHeight="1"/>
+    <row r="166" ht="32.25" customHeight="1"/>
+    <row r="167" ht="32.25" customHeight="1"/>
+    <row r="168" ht="32.25" customHeight="1"/>
+    <row r="169" ht="32.25" customHeight="1"/>
+    <row r="170" ht="32.25" customHeight="1"/>
+    <row r="171" ht="32.25" customHeight="1"/>
+    <row r="172" ht="32.25" customHeight="1"/>
+    <row r="173" ht="32.25" customHeight="1"/>
+    <row r="174" ht="32.25" customHeight="1"/>
+    <row r="175" ht="32.25" customHeight="1"/>
+    <row r="176" ht="32.25" customHeight="1"/>
+    <row r="177" ht="32.25" customHeight="1"/>
+    <row r="178" ht="32.25" customHeight="1"/>
+    <row r="179" ht="32.25" customHeight="1"/>
+    <row r="180" ht="32.25" customHeight="1"/>
+    <row r="181" ht="32.25" customHeight="1"/>
+    <row r="182" ht="32.25" customHeight="1"/>
+    <row r="183" ht="32.25" customHeight="1"/>
+    <row r="184" ht="32.25" customHeight="1"/>
+    <row r="185" ht="32.25" customHeight="1"/>
+    <row r="186" ht="32.25" customHeight="1"/>
+    <row r="187" ht="32.25" customHeight="1"/>
+    <row r="188" ht="32.25" customHeight="1"/>
+    <row r="189" ht="32.25" customHeight="1"/>
+    <row r="190" ht="32.25" customHeight="1"/>
+    <row r="191" ht="32.25" customHeight="1"/>
+    <row r="192" ht="32.25" customHeight="1"/>
+    <row r="193" ht="32.25" customHeight="1"/>
+    <row r="194" ht="32.25" customHeight="1"/>
+    <row r="195" ht="32.25" customHeight="1"/>
+    <row r="196" ht="32.25" customHeight="1"/>
+    <row r="197" ht="32.25" customHeight="1"/>
+    <row r="198" ht="32.25" customHeight="1"/>
+    <row r="199" ht="32.25" customHeight="1"/>
+    <row r="200" ht="32.25" customHeight="1"/>
+    <row r="201" ht="32.25" customHeight="1"/>
+    <row r="202" ht="32.25" customHeight="1"/>
+    <row r="203" ht="32.25" customHeight="1"/>
+    <row r="204" ht="32.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="F4:F10"/>

</xml_diff>